<commit_message>
Revise for changed terminology in data; address inability to knit mosaic plots to PDF
</commit_message>
<xml_diff>
--- a/Data_Export_Query.xlsx
+++ b/Data_Export_Query.xlsx
@@ -419,17 +419,17 @@
       </c>
       <c r="N1" s="0" t="inlineStr">
         <is>
-          <t>Data_Quality_Category</t>
+          <t>Performance_Category</t>
         </is>
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>Data_Quality_Type</t>
+          <t>Performance_Type</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
-          <t>Data_Quality_Timing</t>
+          <t>Performance_Timing</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G17" s="0" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G25" s="0" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G26" s="0" t="inlineStr">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G27" s="0" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G28" s="0" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G29" s="0" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G30" s="0" t="inlineStr">
@@ -1869,16 +1869,6 @@
           <t>Resilience Planning</t>
         </is>
       </c>
-      <c r="F35" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G35" s="0" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
           <t>Erosion</t>
@@ -1920,16 +1910,6 @@
           <t>Resilience Planning</t>
         </is>
       </c>
-      <c r="F36" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G36" s="0" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
       <c r="H36" s="0" t="inlineStr">
         <is>
           <t>Inundation</t>
@@ -1971,16 +1951,6 @@
           <t>Urban Design</t>
         </is>
       </c>
-      <c r="F37" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G37" s="0" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
       <c r="H37" s="0" t="inlineStr">
         <is>
           <t>Erosion</t>
@@ -2022,16 +1992,6 @@
           <t>Urban Design</t>
         </is>
       </c>
-      <c r="F38" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G38" s="0" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
       <c r="H38" s="0" t="inlineStr">
         <is>
           <t>Inundation</t>
@@ -2503,16 +2463,6 @@
           <t>Need user guides! Make models / tools accessible! (visuals with description). Print option.  Video instructions?</t>
         </is>
       </c>
-      <c r="F50" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G50" s="0" t="inlineStr">
-        <is>
-          <t>Aquaculture</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="0">
@@ -2622,7 +2572,7 @@
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G53" s="0" t="inlineStr">
@@ -2673,7 +2623,7 @@
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G54" s="0" t="inlineStr">
@@ -2724,7 +2674,7 @@
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G55" s="0" t="inlineStr">
@@ -2775,7 +2725,7 @@
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G56" s="0" t="inlineStr">
@@ -2826,7 +2776,7 @@
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G57" s="0" t="inlineStr">
@@ -2877,7 +2827,7 @@
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G58" s="0" t="inlineStr">
@@ -2928,7 +2878,7 @@
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G59" s="0" t="inlineStr">
@@ -2979,7 +2929,7 @@
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G60" s="0" t="inlineStr">
@@ -3114,16 +3064,6 @@
           <t>Harbor Design</t>
         </is>
       </c>
-      <c r="F63" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G63" s="0" t="inlineStr">
-        <is>
-          <t>Fishing</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="0">
@@ -3149,16 +3089,6 @@
           <t>Urban Design</t>
         </is>
       </c>
-      <c r="F64" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G64" s="0" t="inlineStr">
-        <is>
-          <t>Fishing</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="0">
@@ -3186,7 +3116,7 @@
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Customizable</t>
         </is>
       </c>
       <c r="G65" s="0" t="inlineStr">
@@ -4135,16 +4065,6 @@
           <t>Resilience Planning</t>
         </is>
       </c>
-      <c r="F85" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G85" s="0" t="inlineStr">
-        <is>
-          <t>Forensics</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="0">
@@ -4170,16 +4090,6 @@
           <t>Urban Design</t>
         </is>
       </c>
-      <c r="F86" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G86" s="0" t="inlineStr">
-        <is>
-          <t>Forensics</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="87">
       <c r="A87" s="0">
@@ -4618,7 +4528,7 @@
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G97" s="0" t="inlineStr">
@@ -4952,7 +4862,7 @@
       </c>
       <c r="F105" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G105" s="0" t="inlineStr">
@@ -5054,7 +4964,7 @@
       </c>
       <c r="F107" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G107" s="0" t="inlineStr">
@@ -5105,7 +5015,7 @@
       </c>
       <c r="F108" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G108" s="0" t="inlineStr">
@@ -5156,7 +5066,7 @@
       </c>
       <c r="F109" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G109" s="0" t="inlineStr">
@@ -5207,7 +5117,7 @@
       </c>
       <c r="F110" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G110" s="0" t="inlineStr">
@@ -5554,7 +5464,7 @@
       </c>
       <c r="F118" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G118" s="0" t="inlineStr">
@@ -5605,7 +5515,7 @@
       </c>
       <c r="F119" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G119" s="0" t="inlineStr">
@@ -5656,7 +5566,7 @@
       </c>
       <c r="F120" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G120" s="0" t="inlineStr">
@@ -6053,7 +5963,7 @@
       </c>
       <c r="F132" s="0" t="inlineStr">
         <is>
-          <t>Help the User</t>
+          <t>Help Users</t>
         </is>
       </c>
       <c r="G132" s="0" t="inlineStr">
@@ -6194,7 +6104,7 @@
       </c>
       <c r="J136" s="0" t="inlineStr">
         <is>
-          <t>Ice models</t>
+          <t>Ice Models</t>
         </is>
       </c>
       <c r="K136" s="0">
@@ -6243,7 +6153,7 @@
       </c>
       <c r="J137" s="0" t="inlineStr">
         <is>
-          <t>Ice models</t>
+          <t>Ice Models</t>
         </is>
       </c>
       <c r="K137" s="0">
@@ -7080,7 +6990,7 @@
       </c>
       <c r="F158" s="0" t="inlineStr">
         <is>
-          <t>Warnings or Alerts</t>
+          <t>Warnings</t>
         </is>
       </c>
       <c r="G158" s="0" t="inlineStr">
@@ -7345,16 +7255,6 @@
           <t>Resilience Planning</t>
         </is>
       </c>
-      <c r="F165" s="0" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="G165" s="0" t="inlineStr">
-        <is>
-          <t>Forensics</t>
-        </is>
-      </c>
     </row>
     <row outlineLevel="0" r="166">
       <c r="A166" s="0">
@@ -11200,7 +11100,7 @@
       </c>
       <c r="J272" s="0" t="inlineStr">
         <is>
-          <t>Ice models</t>
+          <t>Ice Models</t>
         </is>
       </c>
       <c r="K272" s="0">
@@ -11241,7 +11141,7 @@
       </c>
       <c r="J273" s="0" t="inlineStr">
         <is>
-          <t>Ice models</t>
+          <t>Ice Models</t>
         </is>
       </c>
       <c r="K273" s="0">
@@ -11282,7 +11182,7 @@
       </c>
       <c r="J274" s="0" t="inlineStr">
         <is>
-          <t>Ice models</t>
+          <t>Ice Models</t>
         </is>
       </c>
       <c r="K274" s="0">

</xml_diff>